<commit_message>
Fix Static Function Type, Unit Tests
- Fix the type of static function fields to use the type given by decltype(T::func), cannot use std::pair for this, moved to TypePair struct
- Fix the IsFunction condition to account for static functions whose types no longer equate to their pointers
- Complete unit tests reflection refactor
</commit_message>
<xml_diff>
--- a/Field Identification.xlsx
+++ b/Field Identification.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="360" yWindow="60" windowWidth="13395" windowHeight="3165"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="21">
   <si>
     <t>data</t>
   </si>
@@ -106,7 +106,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="21">
+  <borders count="20">
     <border>
       <left/>
       <right/>
@@ -170,21 +170,6 @@
         <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thick">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thick">
         <color auto="1"/>
       </bottom>
       <diagonal/>
@@ -403,54 +388,54 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -460,8 +445,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -757,10 +742,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -772,17 +757,17 @@
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" thickBot="1"/>
     <row r="2" spans="1:6" ht="16.5" thickTop="1" thickBot="1">
-      <c r="B2" s="23"/>
+      <c r="B2" s="22"/>
       <c r="C2" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="10" t="s">
+      <c r="D2" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="15" t="s">
+      <c r="E2" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="F2" s="16" t="s">
+      <c r="F2" s="15" t="s">
         <v>17</v>
       </c>
     </row>
@@ -793,13 +778,13 @@
       <c r="C3" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="E3" s="20" t="s">
+      <c r="D3" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="F3" s="17"/>
+      <c r="F3" s="16"/>
     </row>
     <row r="4" spans="1:6" ht="15.75">
       <c r="B4" s="3" t="s">
@@ -808,13 +793,13 @@
       <c r="C4" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="E4" s="21" t="s">
+      <c r="D4" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="F4" s="18"/>
+      <c r="F4" s="17"/>
     </row>
     <row r="5" spans="1:6" ht="15.75">
       <c r="B5" s="3" t="s">
@@ -823,13 +808,13 @@
       <c r="C5" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="13" t="s">
+      <c r="D5" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="E5" s="21" t="s">
+      <c r="E5" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="F5" s="18" t="s">
+      <c r="F5" s="17" t="s">
         <v>16</v>
       </c>
     </row>
@@ -840,13 +825,13 @@
       <c r="C6" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="E6" s="21" t="s">
+      <c r="D6" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="E6" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="F6" s="18" t="s">
+      <c r="F6" s="17" t="s">
         <v>19</v>
       </c>
     </row>
@@ -857,13 +842,13 @@
       <c r="C7" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="E7" s="21" t="s">
+      <c r="D7" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="E7" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="F7" s="18" t="s">
+      <c r="F7" s="17" t="s">
         <v>20</v>
       </c>
     </row>
@@ -872,20 +857,21 @@
       <c r="B8" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="D8" s="14" t="s">
-        <v>5</v>
-      </c>
-      <c r="E8" s="22" t="s">
+      <c r="C8" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="E8" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="F8" s="19" t="s">
-        <v>20</v>
-      </c>
+      <c r="F8" s="18"/>
     </row>
     <row r="9" spans="1:6" ht="15.75" thickTop="1"/>
+    <row r="10" spans="1:6" ht="15.75">
+      <c r="F10" s="23"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Update Documentation, Cleanup Main
Update field identification documentation, slight cleanup on example code
</commit_message>
<xml_diff>
--- a/Field Identification.xlsx
+++ b/Field Identification.xlsx
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="FieldIdentification" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -73,10 +73,10 @@
     <t>Example</t>
   </si>
   <si>
-    <t>Field::Pointer is set to decltype(&amp;T::field), field.pointer gets set to nullptr</t>
-  </si>
-  <si>
     <t>Field::Type gets set to decltype(&amp;T::field)</t>
+  </si>
+  <si>
+    <t>Field::Pointer gets set to nullptr_t, field.pointer gets set to nullptr (pointer type is used intermediately, but pointers to static references are not constexpr, hence setting nullptr)</t>
   </si>
 </sst>
 </file>
@@ -745,14 +745,14 @@
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="13.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="68" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="156.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" thickBot="1"/>
@@ -832,7 +832,7 @@
         <v>13</v>
       </c>
       <c r="F6" s="17" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="15.75">
@@ -849,7 +849,7 @@
         <v>14</v>
       </c>
       <c r="F7" s="17" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="16.5" thickBot="1">

</xml_diff>